<commit_message>
feat: make api activated pond
</commit_message>
<xml_diff>
--- a/doc/Sprint04/routes table/routes_table.xlsx
+++ b/doc/Sprint04/routes table/routes_table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrirahmanto/flask/fishapi/doc/Sprint02/routes table/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrirahmanto/flask/fishapi/doc/Sprint04/routes table/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A814AB-5EE1-9C43-BFDB-6D83E5C71B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CC96E5-EED0-BF47-BA78-404C663D7D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{C254AC1B-B4CF-49CB-B06F-3FDC00B6733D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -155,6 +155,33 @@
   </si>
   <si>
     <t>/api/feedhistorysbypond/{pond_id}</t>
+  </si>
+  <si>
+    <t>aktifasi kolam</t>
+  </si>
+  <si>
+    <t>/api/ponds/status</t>
+  </si>
+  <si>
+    <t>/api/ponds/{pond_id}/activation</t>
+  </si>
+  <si>
+    <t>/api/ponds/{pond_id}/diactivation</t>
+  </si>
+  <si>
+    <t>/api/ponds/status/{pond_id}</t>
+  </si>
+  <si>
+    <t>menampilkan aktifasi dan diaktifasi suatu kolam berdasarkan pond_id</t>
+  </si>
+  <si>
+    <t>mengaktifasi suatu kolam berdasarkan pond_id</t>
+  </si>
+  <si>
+    <t>mendiaktifasi suatu kolam berdasarkan pond_id</t>
+  </si>
+  <si>
+    <t>menampilkan aktifasi dan diaktifasi list kolam berdasarkan pond_id</t>
   </si>
 </sst>
 </file>
@@ -170,7 +197,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +228,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -266,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -288,6 +327,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -604,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A9212EE-4B8C-4B45-BD8A-30CF3A593525}">
-  <dimension ref="A2:E21"/>
+  <dimension ref="A2:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -721,170 +774,240 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="15"/>
+      <c r="B12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="15"/>
+      <c r="B13" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="16"/>
+      <c r="B14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="B12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="9"/>
       <c r="B17" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="9"/>
+      <c r="B19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="9"/>
+      <c r="B20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="9"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="9"/>
+      <c r="B22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="10"/>
+      <c r="B23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="4" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="7"/>
+      <c r="B26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A16:A23"/>
+    <mergeCell ref="A11:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: add view list pond activation
</commit_message>
<xml_diff>
--- a/doc/Sprint04/routes table/routes_table.xlsx
+++ b/doc/Sprint04/routes table/routes_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrirahmanto/flask/fishapi/doc/Sprint04/routes table/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CC96E5-EED0-BF47-BA78-404C663D7D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B41E90-B9D4-2043-BBFE-83E83E9BA1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{C254AC1B-B4CF-49CB-B06F-3FDC00B6733D}"/>
   </bookViews>
@@ -314,6 +314,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -329,14 +334,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A9212EE-4B8C-4B45-BD8A-30CF3A593525}">
   <dimension ref="A2:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="135" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -697,7 +697,7 @@
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -714,7 +714,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -729,7 +729,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
@@ -744,7 +744,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
@@ -759,7 +759,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -774,71 +774,71 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="15"/>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="15"/>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="16"/>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="8" t="s">
         <v>47</v>
       </c>
     </row>
@@ -850,7 +850,7 @@
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -867,7 +867,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="3" t="s">
         <v>6</v>
       </c>
@@ -882,7 +882,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
@@ -897,7 +897,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="3" t="s">
         <v>5</v>
       </c>
@@ -912,7 +912,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
@@ -927,14 +927,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="3" t="s">
         <v>17</v>
       </c>
@@ -949,7 +949,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="3" t="s">
         <v>17</v>
       </c>
@@ -971,7 +971,7 @@
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -988,7 +988,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
+      <c r="A26" s="10"/>
       <c r="B26" s="4" t="s">
         <v>17</v>
       </c>

</xml_diff>